<commit_message>
Finished exploratory research: specific to Europe
</commit_message>
<xml_diff>
--- a/Europe_temp_data.xlsx
+++ b/Europe_temp_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agniv\Downloads\UN-Debate-Corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEB737CC-BCE8-4734-A7F7-875E02ECF92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC336B9E-F072-423B-A688-BF7A43478DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2E3C53E-4A46-408D-81EF-0E38066C61A0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A2E3C53E-4A46-408D-81EF-0E38066C61A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,16 +23,24 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Temperature change</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,403 +390,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BC2E9F-3094-4EFC-96BB-3AE8759FF75F}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>1970</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>0.26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>1971</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>1972</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>0.51</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>1973</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>1974</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>0.79</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>1975</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>1.06</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>1976</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>-0.28000000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>1977</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>0.37</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
         <v>1978</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>-0.24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
         <v>1979</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
         <v>1980</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>-0.23</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
         <v>1981</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>0.52</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>1982</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>0.68</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
         <v>1983</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>0.94</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>1984</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>0.42</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
         <v>1985</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>-0.37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>1986</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>1987</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>-0.33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>1988</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>0.73</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>1989</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>1.65</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>1990</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>1.48</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
         <v>1991</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>0.7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
         <v>1992</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>0.9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
         <v>1993</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>0.38</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
         <v>1994</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>1.25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
         <v>1995</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>1.07</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
         <v>1996</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>0.31</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
         <v>1997</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>0.84</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
         <v>1998</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>0.86</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
         <v>1999</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>1.48</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
         <v>2000</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>1.7</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33">
         <v>2001</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <v>1.26</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
         <v>2002</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>1.47</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35">
         <v>2003</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>1.35</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36">
         <v>2004</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>1.2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37">
         <v>2005</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>1.24</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38">
         <v>2006</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>1.4</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39">
         <v>2007</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>1.83</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40">
         <v>2008</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>1.7</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41">
         <v>2009</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>1.48</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42">
         <v>2010</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>0.95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43">
         <v>2011</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>1.7</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44">
         <v>2012</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <v>1.33</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45">
         <v>2013</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>1.56</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46">
         <v>2014</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>2.15</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47">
         <v>2015</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48">
         <v>2016</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <v>1.89</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49">
         <v>2017</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <v>1.85</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50">
         <v>2018</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>2.27</v>
       </c>
     </row>

</xml_diff>